<commit_message>
Add Logo + Comment
</commit_message>
<xml_diff>
--- a/DDC/Config.xlsx
+++ b/DDC/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ProjetDDC\DDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B029C7-23CD-43B0-9922-71A82B51E0BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDB8B41-A59D-4D8E-9C86-67D58B175083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1805,10 +1805,10 @@
         <v>76</v>
       </c>
       <c r="C72" s="4">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D72" s="4">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="2:4">

</xml_diff>